<commit_message>
comit for testing excel sheet
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -5,25 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Settings" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Test Cases" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="Action_Keywords" vbProcedure="false">Settings!$D$2:$D$11</definedName>
-    <definedName function="false" hidden="false" name="Home_Page" vbProcedure="false">Settings!$B$2:$B$11</definedName>
-    <definedName function="false" hidden="false" name="Login_Page" vbProcedure="false">Settings!$C$2:$C$11</definedName>
-    <definedName function="false" hidden="false" name="Page_Name" vbProcedure="false">Settings!$A$2:$A$11</definedName>
+    <definedName function="false" hidden="false" name="Action_Keywords" vbProcedure="false">#ref!!$d$2:$d$11</definedName>
+    <definedName function="false" hidden="false" name="Home_Page" vbProcedure="false">#ref!!$b$2:$b$11</definedName>
+    <definedName function="false" hidden="false" name="Login_Page" vbProcedure="false">#ref!!$c$2:$c$11</definedName>
+    <definedName function="false" hidden="false" name="Page_Name" vbProcedure="false">#ref!!$a$2:$a$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -64,28 +62,43 @@
     <t>Navigate to the Website</t>
   </si>
   <si>
+    <t>user name</t>
+  </si>
+  <si>
     <t>TS_003</t>
   </si>
   <si>
     <t>Click on My Account Button On the top right location</t>
   </si>
   <si>
+    <t>fjhjf</t>
+  </si>
+  <si>
     <t>TS_004</t>
   </si>
   <si>
     <t>Enter the username in the Username field</t>
   </si>
   <si>
+    <t>cnjzc</t>
+  </si>
+  <si>
     <t>TS_005</t>
   </si>
   <si>
     <t>Enter the password in the Password field</t>
   </si>
   <si>
+    <t>xfbj</t>
+  </si>
+  <si>
     <t>TS_006</t>
   </si>
   <si>
     <t>Click on login button</t>
+  </si>
+  <si>
+    <t>vcgh</t>
   </si>
   <si>
     <t>TS_007</t>
@@ -254,8 +267,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F7" activeCellId="0" pane="topLeft" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -327,6 +340,12 @@
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>123445</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -338,10 +357,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>13442</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -354,10 +379,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>23456</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -365,15 +396,21 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>64664</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -381,15 +418,21 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>456789</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -402,10 +445,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -418,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -434,10 +477,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -457,10 +500,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -470,7 +513,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="13">
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -480,7 +523,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="14">
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -490,32 +533,32 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="15">
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="16">
       <c r="C16" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="17">
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="C18" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="C20" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -537,63 +580,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.05"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="18.5765306122449"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="1" s="1"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D4" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.05"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="1" s="1"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>